<commit_message>
route updates and temporary cache for route code
</commit_message>
<xml_diff>
--- a/app/shiny/templates/routes.xlsx
+++ b/app/shiny/templates/routes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\DesktopDeployR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBE3A4A-87AD-4330-858D-8402B831E87B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F69046B-3DB1-483B-AD45-2817C4D1DAB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12390" yWindow="2535" windowWidth="15705" windowHeight="12750" xr2:uid="{69E47BAC-755F-4C59-B0FA-B6A795F816AB}"/>
+    <workbookView xWindow="3300" yWindow="3300" windowWidth="18255" windowHeight="11760" xr2:uid="{69E47BAC-755F-4C59-B0FA-B6A795F816AB}"/>
   </bookViews>
   <sheets>
     <sheet name="routes" sheetId="1" r:id="rId1"/>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5CFF22-F59D-4FE4-86BB-861E90041BD0}">
   <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1334,13 +1334,13 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -1532,13 +1532,13 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
added input for cloth masks and new zip code to routes
</commit_message>
<xml_diff>
--- a/app/shiny/templates/routes.xlsx
+++ b/app/shiny/templates/routes.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\DesktopDeployR\app\shiny\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ppe_allocatoR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F69046B-3DB1-483B-AD45-2817C4D1DAB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836FB1F4-C51C-4FF1-A4A8-0A463416BD3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="3300" windowWidth="18255" windowHeight="11760" xr2:uid="{69E47BAC-755F-4C59-B0FA-B6A795F816AB}"/>
+    <workbookView xWindow="3765" yWindow="720" windowWidth="24840" windowHeight="14325" xr2:uid="{69E47BAC-755F-4C59-B0FA-B6A795F816AB}"/>
   </bookViews>
   <sheets>
     <sheet name="routes" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">routes!$A$1:$C$98</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">routes!$A$1:$C$99</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="114">
   <si>
     <t>Bellevue</t>
   </si>
@@ -470,8 +470,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DE8CAB3-C436-46B5-9C7D-15023E0AE8CB}" name="Routes" displayName="Routes" ref="A1:C98" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C98" xr:uid="{166E2358-DC76-45CD-AFEF-DD20543F0A05}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DE8CAB3-C436-46B5-9C7D-15023E0AE8CB}" name="Routes" displayName="Routes" ref="A1:C99" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C99" xr:uid="{166E2358-DC76-45CD-AFEF-DD20543F0A05}"/>
   <tableColumns count="3">
     <tableColumn id="4" xr3:uid="{F8D3A697-12C4-4343-93A3-8D63116F50D1}" uniqueName="4" name="name" queryTableFieldId="4" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{A8F6A94C-582C-4819-9106-82DC542D9513}" uniqueName="5" name="zip" queryTableFieldId="5" dataDxfId="1"/>
@@ -778,22 +778,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5CFF22-F59D-4FE4-86BB-861E90041BD0}">
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -804,7 +804,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +815,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -826,7 +826,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,7 +837,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,7 +848,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -859,7 +859,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -870,7 +870,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -881,7 +881,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -892,7 +892,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -903,7 +903,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -914,7 +914,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -925,7 +925,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -936,7 +936,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -947,7 +947,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -958,7 +958,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -969,7 +969,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -980,7 +980,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -991,7 +991,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>90</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>29</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>29</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>29</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>29</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>29</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>29</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>55</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>55</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>55</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>55</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>55</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>55</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>55</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>55</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>55</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>55</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>55</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>55</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>55</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>72</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>72</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>72</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>72</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>72</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>72</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>72</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>72</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>72</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>72</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>72</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>72</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>72</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>72</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>90</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>90</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>90</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>90</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>90</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>90</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>90</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>90</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>90</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>90</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>90</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>90</v>
       </c>
@@ -1869,6 +1869,17 @@
       </c>
       <c r="C98" s="1" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" s="1">
+        <v>98288</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 2 ltcfs and updated 3 zip code routes
</commit_message>
<xml_diff>
--- a/app/shiny/templates/routes.xlsx
+++ b/app/shiny/templates/routes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahu.PH\Documents\GitHub\ppe_allocatoR\app\shiny\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ppe_allocatoR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7595B240-C0FF-44AD-9630-C5ADF308BCD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610784A5-43FA-4BBC-92B0-6A08EECA4BAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18160" yWindow="5700" windowWidth="1980" windowHeight="560" xr2:uid="{69E47BAC-755F-4C59-B0FA-B6A795F816AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{69E47BAC-755F-4C59-B0FA-B6A795F816AB}"/>
   </bookViews>
   <sheets>
     <sheet name="routes" sheetId="1" r:id="rId1"/>
@@ -757,19 +757,19 @@
   <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>99</v>
       </c>
@@ -780,7 +780,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -791,7 +791,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -802,7 +802,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -813,7 +813,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -824,7 +824,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -835,7 +835,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -846,7 +846,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -857,7 +857,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -868,7 +868,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -879,7 +879,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -890,7 +890,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -901,7 +901,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -912,7 +912,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -923,7 +923,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -934,7 +934,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -945,7 +945,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -956,7 +956,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -967,7 +967,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -978,7 +978,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -989,7 +989,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>102</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>102</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>102</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>102</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>102</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>102</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>102</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>102</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>102</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>102</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>102</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>102</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>102</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>102</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>102</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>102</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>102</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>102</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>104</v>
       </c>
@@ -1283,10 +1283,10 @@
         <v>47</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>7</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -1308,18 +1308,18 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>104</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>104</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>104</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>104</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>104</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>104</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>104</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>104</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>104</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>104</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>104</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>104</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>104</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>104</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>104</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>104</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>104</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>104</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>104</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>104</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>104</v>
       </c>
@@ -1561,18 +1561,18 @@
         <v>105</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>104</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>104</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>104</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>104</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>104</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>104</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>104</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>104</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>104</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>104</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>104</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>102</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>102</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>102</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>102</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>102</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>102</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>102</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>102</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>102</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>102</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>102</v>
       </c>
@@ -1814,18 +1814,18 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>95</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>102</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>102</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
update ltcf case files
updates to accommodate formatting of cases file for ltcfs
</commit_message>
<xml_diff>
--- a/app/shiny/templates/routes.xlsx
+++ b/app/shiny/templates/routes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahu.PH\Documents\GitHub\ppe_allocatoR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7595B240-C0FF-44AD-9630-C5ADF308BCD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931FC129-21D9-4679-AB89-94B5287A651F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18160" yWindow="5700" windowWidth="1980" windowHeight="560" xr2:uid="{69E47BAC-755F-4C59-B0FA-B6A795F816AB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{69E47BAC-755F-4C59-B0FA-B6A795F816AB}"/>
   </bookViews>
   <sheets>
     <sheet name="routes" sheetId="1" r:id="rId1"/>
@@ -757,7 +757,7 @@
   <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1294,7 +1294,7 @@
         <v>48</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1310,7 +1310,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>50</v>
@@ -1563,13 +1563,13 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -1624,7 +1624,7 @@
         <v>78</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -1635,7 +1635,7 @@
         <v>79</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -1668,7 +1668,7 @@
         <v>82</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -1679,7 +1679,7 @@
         <v>83</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -1816,7 +1816,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>95</v>

</xml_diff>